<commit_message>
Corrigindo ID e Rastreabilidade
Corrigindo ID dos requisitos no documento de especificação e na matriz
de rastreabilidade; Revisando matriz de rastreabilidade
</commit_message>
<xml_diff>
--- a/Documentos de especificação complementar/Matriz de Rastreabilidade.xlsx
+++ b/Documentos de especificação complementar/Matriz de Rastreabilidade.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\ENG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Projeto Engenharia de Software II\Documentos de especificação complementar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de Rastreabilidade" sheetId="1" r:id="rId1"/>
@@ -24,27 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Alvo</t>
   </si>
   <si>
     <t>Fonte</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
-    <t>F5</t>
   </si>
   <si>
     <t>R</t>
@@ -59,7 +44,25 @@
     <t>Relacionado</t>
   </si>
   <si>
-    <t>F6</t>
+    <t>ADDT</t>
+  </si>
+  <si>
+    <t>DELT</t>
+  </si>
+  <si>
+    <t>ALTT</t>
+  </si>
+  <si>
+    <t>VILT</t>
+  </si>
+  <si>
+    <t>ORDT</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>Vazio</t>
   </si>
 </sst>
 </file>
@@ -116,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -155,19 +158,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -400,42 +390,62 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,14 +453,49 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -468,6 +513,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -824,346 +889,353 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="3.5703125" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
-    </row>
-    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="O3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="P3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
+    </row>
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+      <c r="O4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="11" t="s">
+    </row>
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="12"/>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
-      <c r="O3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="8" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
-      <c r="O4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-      <c r="S8" s="5"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
+      <c r="S8" s="4"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="14"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="19"/>
     </row>
     <row r="18" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="16"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1189,27 +1261,24 @@
     <mergeCell ref="B1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:M18">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="O3:O4">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"R"</formula>
+  <conditionalFormatting sqref="C3:M18 O5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/ALREstevam/SI304B-ProjetoEngenhariaII"
This reverts commit 2c29ff968f0d37b4d3ab62a3be37303f200e154f, reversing
changes made to 2191fa1d09c47e0ecdc80ab8b33caebdcb6fffcf.
</commit_message>
<xml_diff>
--- a/Documentos de especificação complementar/Matriz de Rastreabilidade.xlsx
+++ b/Documentos de especificação complementar/Matriz de Rastreabilidade.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Projeto Engenharia de Software II\Documentos de especificação complementar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\ENG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de Rastreabilidade" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>Alvo</t>
   </si>
   <si>
     <t>Fonte</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
   </si>
   <si>
     <t>R</t>
@@ -44,25 +59,7 @@
     <t>Relacionado</t>
   </si>
   <si>
-    <t>ADDT</t>
-  </si>
-  <si>
-    <t>DELT</t>
-  </si>
-  <si>
-    <t>ALTT</t>
-  </si>
-  <si>
-    <t>VILT</t>
-  </si>
-  <si>
-    <t>ORDT</t>
-  </si>
-  <si>
-    <t>COLOR</t>
-  </si>
-  <si>
-    <t>Vazio</t>
+    <t>F6</t>
   </si>
 </sst>
 </file>
@@ -119,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -158,6 +155,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -390,62 +400,42 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -453,49 +443,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -513,26 +468,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -889,353 +824,346 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="3.5703125" customWidth="1"/>
+    <col min="2" max="13" width="3.5703125" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:19" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+    </row>
+    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="H2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
+      <c r="O3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="P3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="16" t="s">
+    </row>
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="O4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="16" t="s">
+    </row>
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="17"/>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
-      <c r="O3" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="6" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="19"/>
-      <c r="O4" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="P4" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="19"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="19"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="19"/>
-      <c r="S8" s="4"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
+      <c r="S8" s="5"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="19"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="19"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="19"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="19"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="19"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="19"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="19"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="14"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="19"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
     </row>
     <row r="18" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="21"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1261,24 +1189,27 @@
     <mergeCell ref="B1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:M18">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O4">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+  <conditionalFormatting sqref="O3">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:M18 O5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>0</formula>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/ALREstevam/SI304B-ProjetoEngenhariaII""
This reverts commit cadd2c47c7241c032b64d9ed0b56b3fcc9771bfe.
</commit_message>
<xml_diff>
--- a/Documentos de especificação complementar/Matriz de Rastreabilidade.xlsx
+++ b/Documentos de especificação complementar/Matriz de Rastreabilidade.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\ENG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Projeto Engenharia de Software II\Documentos de especificação complementar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8115"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de Rastreabilidade" sheetId="1" r:id="rId1"/>
@@ -24,27 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Alvo</t>
   </si>
   <si>
     <t>Fonte</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
-    <t>F5</t>
   </si>
   <si>
     <t>R</t>
@@ -59,7 +44,25 @@
     <t>Relacionado</t>
   </si>
   <si>
-    <t>F6</t>
+    <t>ADDT</t>
+  </si>
+  <si>
+    <t>DELT</t>
+  </si>
+  <si>
+    <t>ALTT</t>
+  </si>
+  <si>
+    <t>VILT</t>
+  </si>
+  <si>
+    <t>ORDT</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>Vazio</t>
   </si>
 </sst>
 </file>
@@ -116,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -155,19 +158,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -400,42 +390,62 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,14 +453,49 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -468,6 +513,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -824,346 +889,353 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="3.5703125" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
-    </row>
-    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="17"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="O3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="P3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
+    </row>
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
+      <c r="O4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="11" t="s">
+    </row>
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="12"/>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
-      <c r="O3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="8" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
-      <c r="O4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
-      <c r="S8" s="5"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
+      <c r="S8" s="4"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="14"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="19"/>
     </row>
     <row r="18" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="16"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1189,27 +1261,24 @@
     <mergeCell ref="B1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:M18">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="O3:O4">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"D"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"R"</formula>
+  <conditionalFormatting sqref="C3:M18 O5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>